<commit_message>
I did a thing
</commit_message>
<xml_diff>
--- a/Migration-Simulator/main_data/job_opportunities.xlsx
+++ b/Migration-Simulator/main_data/job_opportunities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/66433c94f25ee271/Desktop/Kanti Baden/Maturaarbeit/MigrationBaden/Migration-Simulator/main_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="11_71DE19FB0A387E79B9319077F863A18F3CF0A445" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93D740B2-CF27-463E-A610-84CF74B5D265}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="11_71DE19FB0A387E79B9319077F863A18F3CF0A445" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AB7EFB9-4AC9-4E69-A7D1-3CA9545DFAC4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>BFS
 Nummer</t>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>Wuerenlos</t>
-  </si>
-  <si>
-    <t>sss</t>
   </si>
 </sst>
 </file>
@@ -667,7 +664,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -698,7 +695,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="17" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="60">
     <cellStyle name="20 % - Akzent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1065,7 +1061,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -1987,9 +1983,7 @@
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C32" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="C32" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>